<commit_message>
IDEFICS-5 changed conversion number in tg, chol, hdl and ldl slightly to be consistent with EPICP
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_IDEFICS_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_IDEFICS_INES.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C99011-3A3F-48DE-B499-0CAFAE4AC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -368,28 +374,28 @@
 na_day (Core)</t>
   </si>
   <si>
-    <t>trg * 0.0113</t>
-  </si>
-  <si>
-    <t>tc * 0.0259</t>
-  </si>
-  <si>
-    <t>ldl * 0.0259</t>
-  </si>
-  <si>
-    <t>hdl* 0.0259</t>
-  </si>
-  <si>
     <t>Sodium intake [mg/d]</t>
   </si>
   <si>
     <t>Sodium to potassium intake ratio</t>
+  </si>
+  <si>
+    <t>trg/88.57</t>
+  </si>
+  <si>
+    <t>tc/38.67</t>
+  </si>
+  <si>
+    <t>ldl/38.67</t>
+  </si>
+  <si>
+    <t>hdl/38.67</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,9 +510,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -544,9 +550,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,7 +587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -616,7 +622,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -789,21 +795,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.81640625" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -858,7 +868,7 @@
         <v>82</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="3" t="s">
@@ -868,7 +878,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -888,7 +898,7 @@
         <v>82</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="3" t="s">
@@ -898,7 +908,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -918,7 +928,7 @@
         <v>82</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="3" t="s">
@@ -928,7 +938,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -948,7 +958,7 @@
         <v>82</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="3" t="s">
@@ -958,7 +968,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -988,7 +998,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -1018,7 +1028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
@@ -1035,7 +1045,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1062,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1092,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -1112,7 +1122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -1142,7 +1152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -1170,7 +1180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -1198,7 +1208,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>40</v>
       </c>
@@ -1228,7 +1238,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>42</v>
       </c>
@@ -1242,7 +1252,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
@@ -1256,7 +1266,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1286,7 +1296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1326,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1346,7 +1356,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>52</v>
       </c>
@@ -1406,7 +1416,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>54</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>56</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1506,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>60</v>
       </c>
@@ -1526,7 +1536,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>62</v>
       </c>
@@ -1556,7 +1566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>64</v>
       </c>
@@ -1586,7 +1596,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -1613,7 +1623,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -1640,7 +1650,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -1670,7 +1680,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -1700,7 +1710,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -1754,12 +1764,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="2:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>13</v>
@@ -1783,12 +1793,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>13</v>

</xml_diff>